<commit_message>
Update excel manual test cases
</commit_message>
<xml_diff>
--- a/Saucedemo Test Cases.xlsx
+++ b/Saucedemo Test Cases.xlsx
@@ -1578,7 +1578,7 @@
         <color rgb="FF000000"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">User is logged in, added products in cart and is on </t>
+      <t xml:space="preserve">User is logged in, has added products in cart and is on </t>
     </r>
     <r>
       <rPr>
@@ -1657,7 +1657,7 @@
         <color rgb="FF000000"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">User is logged in, added products in cart and is on </t>
+      <t xml:space="preserve">User is logged in, has added products in cart and is on </t>
     </r>
     <r>
       <rPr>
@@ -1736,7 +1736,7 @@
         <color rgb="FF000000"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">User is logged in, added products in cart and is on </t>
+      <t xml:space="preserve">User is logged in, has added products in cart and is on </t>
     </r>
     <r>
       <rPr>
@@ -1815,7 +1815,7 @@
         <color rgb="FF000000"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">User is logged in, added products in cart and is on </t>
+      <t xml:space="preserve">User is logged in, has added products in cart and is on </t>
     </r>
     <r>
       <rPr>
@@ -1894,7 +1894,7 @@
         <color rgb="FF000000"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">User is logged in, added products in cart and is on </t>
+      <t xml:space="preserve">User is logged in, has added products in cart and is on </t>
     </r>
     <r>
       <rPr>
@@ -1967,7 +1967,7 @@
     <t>Verify that "Item total" is sum of all products prices in cart</t>
   </si>
   <si>
-    <t>User is logged in, added products in cart and filled checkout form</t>
+    <t>User is logged in, has added products in cart and filled checkout form</t>
   </si>
   <si>
     <t>1. User clicks on "Continue" button</t>
@@ -2088,7 +2088,7 @@
         <color rgb="FF000000"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">User is logged in, added products in cart, filled checkout form and is on </t>
+      <t xml:space="preserve">User is logged in, has added products in cart, filled checkout form and is on </t>
     </r>
     <r>
       <rPr>

</xml_diff>